<commit_message>
debug plants risk score script - 2 more correct (change implementation of nt + mt)
</commit_message>
<xml_diff>
--- a/Arable_plant_requirements.xlsx
+++ b/Arable_plant_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA700E8-AF0E-C746-8B9A-79E6AA87687B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220CAF07-1EE6-7E48-AB5F-B3862B19244F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL SPECIES'!$A$2:$AQ$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL SPECIES'!$A$1:$AR$190</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1533,10 +1533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="O9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1555,17 +1556,17 @@
     <col min="13" max="13" width="17.5" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="9.1640625" style="55" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="27" customWidth="1"/>
+    <col min="18" max="18" width="19" style="10" customWidth="1"/>
+    <col min="19" max="19" width="19.5" style="10" customWidth="1"/>
+    <col min="20" max="20" width="18.5" style="10" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" style="27" customWidth="1"/>
+    <col min="22" max="22" width="19.5" style="10" customWidth="1"/>
+    <col min="23" max="23" width="19.83203125" style="10" customWidth="1"/>
+    <col min="24" max="24" width="19" style="10" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" style="27" customWidth="1"/>
+    <col min="26" max="26" width="19" style="10" customWidth="1"/>
+    <col min="27" max="27" width="19.5" style="10" customWidth="1"/>
     <col min="28" max="28" width="18.5" style="10" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="9.1640625" style="55" customWidth="1"/>
     <col min="31" max="31" width="13.5" style="28" bestFit="1" customWidth="1"/>
@@ -1770,7 +1771,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>39</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -3354,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
@@ -3453,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>51</v>
       </c>
@@ -3750,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>52</v>
       </c>
@@ -3849,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
@@ -3948,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>54</v>
       </c>
@@ -4047,7 +4048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>55</v>
       </c>
@@ -4146,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>56</v>
       </c>
@@ -4245,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>58</v>
       </c>
@@ -4443,7 +4444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>59</v>
       </c>
@@ -4542,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>60</v>
       </c>
@@ -4641,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
@@ -4839,7 +4840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>63</v>
       </c>
@@ -4938,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>64</v>
       </c>
@@ -5037,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>65</v>
       </c>
@@ -5136,7 +5137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>66</v>
       </c>
@@ -5334,7 +5335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>68</v>
       </c>
@@ -5433,7 +5434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>69</v>
       </c>
@@ -5532,7 +5533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>70</v>
       </c>
@@ -5730,7 +5731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>72</v>
       </c>
@@ -5829,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>73</v>
       </c>
@@ -5928,7 +5929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>74</v>
       </c>
@@ -6027,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>75</v>
       </c>
@@ -6126,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>76</v>
       </c>
@@ -6225,7 +6226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>77</v>
       </c>
@@ -6324,7 +6325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>78</v>
       </c>
@@ -6423,7 +6424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>79</v>
       </c>
@@ -6522,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>80</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>81</v>
       </c>
@@ -6720,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>82</v>
       </c>
@@ -6819,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>83</v>
       </c>
@@ -6918,7 +6919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>84</v>
       </c>
@@ -7116,7 +7117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>86</v>
       </c>
@@ -7215,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>87</v>
       </c>
@@ -7314,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>88</v>
       </c>
@@ -7413,7 +7414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>89</v>
       </c>
@@ -7512,7 +7513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>90</v>
       </c>
@@ -7611,7 +7612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>91</v>
       </c>
@@ -7809,7 +7810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>93</v>
       </c>
@@ -7908,7 +7909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>94</v>
       </c>
@@ -8007,7 +8008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>95</v>
       </c>
@@ -8106,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>96</v>
       </c>
@@ -8403,7 +8404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>99</v>
       </c>
@@ -8502,7 +8503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
         <v>100</v>
       </c>
@@ -8601,7 +8602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>101</v>
       </c>
@@ -8700,7 +8701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>102</v>
       </c>
@@ -8799,7 +8800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>103</v>
       </c>
@@ -8898,7 +8899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>104</v>
       </c>
@@ -8997,7 +8998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>105</v>
       </c>
@@ -9096,7 +9097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>106</v>
       </c>
@@ -9294,7 +9295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>108</v>
       </c>
@@ -9393,7 +9394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>109</v>
       </c>
@@ -9492,7 +9493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>110</v>
       </c>
@@ -9591,7 +9592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>111</v>
       </c>
@@ -9690,7 +9691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>112</v>
       </c>
@@ -9789,7 +9790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>113</v>
       </c>
@@ -9888,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>114</v>
       </c>
@@ -9987,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>115</v>
       </c>
@@ -10086,7 +10087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:43" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:43" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>116</v>
       </c>
@@ -10185,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>117</v>
       </c>
@@ -10284,7 +10285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>118</v>
       </c>
@@ -10383,7 +10384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="s">
         <v>119</v>
       </c>
@@ -10482,7 +10483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>120</v>
       </c>
@@ -10581,7 +10582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>121</v>
       </c>
@@ -10680,7 +10681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>122</v>
       </c>
@@ -10779,7 +10780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>123</v>
       </c>
@@ -10878,7 +10879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>124</v>
       </c>
@@ -10977,7 +10978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>125</v>
       </c>
@@ -11076,7 +11077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>126</v>
       </c>
@@ -11175,7 +11176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>127</v>
       </c>
@@ -11274,7 +11275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>128</v>
       </c>
@@ -11373,7 +11374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>129</v>
       </c>
@@ -11472,7 +11473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="s">
         <v>130</v>
       </c>
@@ -11571,7 +11572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:43" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:43" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>131</v>
       </c>
@@ -11670,7 +11671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>132</v>
       </c>
@@ -11769,7 +11770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>133</v>
       </c>
@@ -12066,7 +12067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>136</v>
       </c>
@@ -12165,7 +12166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
         <v>137</v>
       </c>
@@ -12264,7 +12265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>138</v>
       </c>
@@ -12363,7 +12364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>139</v>
       </c>
@@ -12462,7 +12463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>140</v>
       </c>
@@ -12759,7 +12760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>143</v>
       </c>
@@ -12858,7 +12859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>144</v>
       </c>
@@ -12957,7 +12958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>145</v>
       </c>
@@ -13056,7 +13057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>146</v>
       </c>
@@ -13155,7 +13156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>147</v>
       </c>
@@ -13254,7 +13255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>148</v>
       </c>
@@ -13353,7 +13354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>149</v>
       </c>
@@ -13452,7 +13453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>150</v>
       </c>
@@ -13551,7 +13552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>151</v>
       </c>
@@ -13650,7 +13651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>152</v>
       </c>
@@ -13749,7 +13750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>153</v>
       </c>
@@ -13848,7 +13849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
         <v>154</v>
       </c>
@@ -13947,7 +13948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>155</v>
       </c>
@@ -14046,7 +14047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>156</v>
       </c>
@@ -14145,7 +14146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>157</v>
       </c>
@@ -14244,7 +14245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
         <v>158</v>
       </c>
@@ -14343,7 +14344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>159</v>
       </c>
@@ -14442,7 +14443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>160</v>
       </c>
@@ -14640,7 +14641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>162</v>
       </c>
@@ -14739,7 +14740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>163</v>
       </c>
@@ -14838,7 +14839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>164</v>
       </c>
@@ -15036,7 +15037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>166</v>
       </c>
@@ -15135,7 +15136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="s">
         <v>167</v>
       </c>
@@ -15234,7 +15235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>168</v>
       </c>
@@ -15333,7 +15334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
         <v>169</v>
       </c>
@@ -15432,7 +15433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>170</v>
       </c>
@@ -15531,7 +15532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>171</v>
       </c>
@@ -15630,7 +15631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>172</v>
       </c>
@@ -15729,7 +15730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>173</v>
       </c>
@@ -15828,7 +15829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>174</v>
       </c>
@@ -16026,7 +16027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>176</v>
       </c>
@@ -16125,7 +16126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="12" t="s">
         <v>177</v>
       </c>
@@ -16224,7 +16225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
         <v>178</v>
       </c>
@@ -16323,7 +16324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
         <v>179</v>
       </c>
@@ -16422,7 +16423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>180</v>
       </c>
@@ -16521,7 +16522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>181</v>
       </c>
@@ -16620,7 +16621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>182</v>
       </c>
@@ -16719,7 +16720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>183</v>
       </c>
@@ -16818,7 +16819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
         <v>184</v>
       </c>
@@ -16917,7 +16918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
         <v>185</v>
       </c>
@@ -17016,7 +17017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="12" t="s">
         <v>186</v>
       </c>
@@ -17115,7 +17116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
         <v>187</v>
       </c>
@@ -17214,7 +17215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="12" t="s">
         <v>188</v>
       </c>
@@ -17412,7 +17413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
         <v>190</v>
       </c>
@@ -17511,7 +17512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
         <v>191</v>
       </c>
@@ -17610,7 +17611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
         <v>192</v>
       </c>
@@ -17709,7 +17710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
         <v>193</v>
       </c>
@@ -17808,7 +17809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
         <v>194</v>
       </c>
@@ -17907,7 +17908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
         <v>195</v>
       </c>
@@ -18006,7 +18007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
         <v>196</v>
       </c>
@@ -18105,7 +18106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
         <v>197</v>
       </c>
@@ -18204,7 +18205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
         <v>198</v>
       </c>
@@ -18501,7 +18502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
         <v>201</v>
       </c>
@@ -18600,7 +18601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
         <v>202</v>
       </c>
@@ -18699,7 +18700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
         <v>203</v>
       </c>
@@ -18798,7 +18799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
         <v>204</v>
       </c>
@@ -18897,7 +18898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
         <v>205</v>
       </c>
@@ -18996,7 +18997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
         <v>206</v>
       </c>
@@ -19095,7 +19096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
         <v>207</v>
       </c>
@@ -19194,7 +19195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>208</v>
       </c>
@@ -19293,7 +19294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
         <v>209</v>
       </c>
@@ -19392,7 +19393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
         <v>210</v>
       </c>
@@ -19590,7 +19591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
         <v>212</v>
       </c>
@@ -19689,7 +19690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
         <v>213</v>
       </c>
@@ -19887,7 +19888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>215</v>
       </c>
@@ -19986,7 +19987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
         <v>216</v>
       </c>
@@ -20085,7 +20086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
         <v>217</v>
       </c>
@@ -20184,7 +20185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>218</v>
       </c>
@@ -20383,6 +20384,63 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AR190" xr:uid="{4E863BDD-F346-1648-BFCC-763B278D18B9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Adonis annua"/>
+        <filter val="Alyssum alyssoides"/>
+        <filter val="Anthriscus caucalis"/>
+        <filter val="Aphenes arvensis"/>
+        <filter val="Atriplex prostrata"/>
+        <filter val="Centaurea cyanus"/>
+        <filter val="Chamaenerion angustifolium"/>
+        <filter val="Chrysanthemum segetum"/>
+        <filter val="Epilobium montanum"/>
+        <filter val="Euphorbia platyphyllos"/>
+        <filter val="Filago pyramidata"/>
+        <filter val="Filago vulgaris"/>
+        <filter val="Galium tricornutum"/>
+        <filter val="Medicago arabica"/>
+        <filter val="Medicago lupilina"/>
+        <filter val="Odontites verna"/>
+        <filter val="Papaver dubium"/>
+        <filter val="Scandix pecten-veneris"/>
+        <filter val="Sherardia arvensis"/>
+        <filter val="Sonchus arvensis"/>
+        <filter val="Species"/>
+        <filter val="Torilis arvensis"/>
+        <filter val="Valerianella dentata"/>
+        <filter val="Valerianella rimosa"/>
+        <filter val="Veronica triphyllos"/>
+        <filter val="Vicia sativa"/>
+        <filter val="Viola tricolor"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="17" showButton="0"/>
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <filterColumn colId="20" showButton="0"/>
+    <filterColumn colId="21" showButton="0"/>
+    <filterColumn colId="22" showButton="0"/>
+    <filterColumn colId="23" showButton="0"/>
+    <filterColumn colId="24" showButton="0"/>
+    <filterColumn colId="25" showButton="0"/>
+    <filterColumn colId="26" showButton="0"/>
+    <filterColumn colId="30" showButton="0"/>
+    <filterColumn colId="31" showButton="0"/>
+    <filterColumn colId="35" showButton="0"/>
+    <filterColumn colId="36" showButton="0"/>
+    <filterColumn colId="40" showButton="0"/>
+    <filterColumn colId="41" showButton="0"/>
+  </autoFilter>
   <mergeCells count="6">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="I1:N1"/>

</xml_diff>

<commit_message>
change strat 2 (adding fertiliser) to just cropped hab not all habs
</commit_message>
<xml_diff>
--- a/Arable_plant_requirements.xlsx
+++ b/Arable_plant_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220CAF07-1EE6-7E48-AB5F-B3862B19244F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33949414-2C46-FF4C-A360-61633C303BC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="269">
   <si>
     <t>Species</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Ballota nigra</t>
-  </si>
-  <si>
-    <t>Barbarea vulgaris</t>
   </si>
   <si>
     <t>Bellis perennis</t>
@@ -1533,11 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="O9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1585,14 +1581,14 @@
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="D1" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
       <c r="I1" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -1602,7 +1598,7 @@
       <c r="O1" s="53"/>
       <c r="P1" s="53"/>
       <c r="Q1" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
@@ -1618,21 +1614,21 @@
       <c r="AC1" s="53"/>
       <c r="AD1" s="53"/>
       <c r="AE1" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF1" s="35"/>
       <c r="AG1" s="35"/>
       <c r="AH1" s="53"/>
       <c r="AI1" s="53"/>
       <c r="AJ1" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AK1" s="40"/>
       <c r="AL1" s="40"/>
       <c r="AM1" s="53"/>
       <c r="AN1" s="53"/>
       <c r="AO1" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AP1" s="48"/>
       <c r="AQ1" s="48"/>
@@ -1645,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>2</v>
@@ -1657,10 +1653,10 @@
         <v>4</v>
       </c>
       <c r="G2" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" s="54" t="s">
         <v>259</v>
-      </c>
-      <c r="H2" s="54" t="s">
-        <v>260</v>
       </c>
       <c r="I2" s="30" t="s">
         <v>5</v>
@@ -1681,10 +1677,10 @@
         <v>10</v>
       </c>
       <c r="O2" s="54" t="s">
+        <v>260</v>
+      </c>
+      <c r="P2" s="54" t="s">
         <v>261</v>
-      </c>
-      <c r="P2" s="54" t="s">
-        <v>262</v>
       </c>
       <c r="Q2" s="26" t="s">
         <v>11</v>
@@ -1723,10 +1719,10 @@
         <v>22</v>
       </c>
       <c r="AC2" s="54" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD2" s="54" t="s">
         <v>263</v>
-      </c>
-      <c r="AD2" s="54" t="s">
-        <v>264</v>
       </c>
       <c r="AE2" s="36" t="s">
         <v>23</v>
@@ -1738,10 +1734,10 @@
         <v>25</v>
       </c>
       <c r="AH2" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="AI2" s="54" t="s">
         <v>265</v>
-      </c>
-      <c r="AI2" s="54" t="s">
-        <v>266</v>
       </c>
       <c r="AJ2" s="41" t="s">
         <v>26</v>
@@ -1753,10 +1749,10 @@
         <v>28</v>
       </c>
       <c r="AM2" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="AN2" s="54" t="s">
         <v>267</v>
-      </c>
-      <c r="AN2" s="54" t="s">
-        <v>268</v>
       </c>
       <c r="AO2" s="44" t="s">
         <v>29</v>
@@ -1768,10 +1764,10 @@
         <v>31</v>
       </c>
       <c r="AR2" s="56" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
@@ -1969,7 +1965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
@@ -2167,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -2266,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -2464,7 +2460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>39</v>
       </c>
@@ -2563,7 +2559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
@@ -2662,7 +2658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
@@ -2860,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
@@ -3058,7 +3054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:44" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -3157,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -3256,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -3355,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
@@ -3454,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
@@ -3652,7 +3648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>51</v>
       </c>
@@ -3751,9 +3747,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="8">
         <v>2</v>
@@ -3850,9 +3846,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="8">
         <v>3</v>
@@ -3949,9 +3945,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="8">
         <v>1</v>
@@ -4048,9 +4044,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="8">
         <v>2</v>
@@ -4147,9 +4143,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="8">
         <v>3</v>
@@ -4246,9 +4242,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="8">
         <v>1</v>
@@ -4345,9 +4341,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="8">
         <v>3</v>
@@ -4444,9 +4440,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="8">
         <v>3</v>
@@ -4543,9 +4539,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="8">
         <v>3</v>
@@ -4642,9 +4638,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="8">
         <v>2</v>
@@ -4743,7 +4739,7 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="13">
         <v>1</v>
@@ -4840,9 +4836,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="8">
         <v>3</v>
@@ -4939,9 +4935,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="8">
         <v>3</v>
@@ -5038,9 +5034,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="8">
         <v>3</v>
@@ -5137,9 +5133,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="8">
         <v>3</v>
@@ -5238,7 +5234,7 @@
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="8">
         <v>3</v>
@@ -5335,9 +5331,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="8">
         <v>1</v>
@@ -5434,9 +5430,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="8">
         <v>2</v>
@@ -5533,9 +5529,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="8">
         <v>1</v>
@@ -5634,7 +5630,7 @@
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="8">
         <v>2</v>
@@ -5731,9 +5727,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="8">
         <v>2</v>
@@ -5830,9 +5826,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="8">
         <v>2</v>
@@ -5929,9 +5925,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="8">
         <v>2</v>
@@ -6028,9 +6024,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="8">
         <v>3</v>
@@ -6127,9 +6123,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="8">
         <v>2</v>
@@ -6226,9 +6222,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="8">
         <v>2</v>
@@ -6325,9 +6321,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="8">
         <v>1</v>
@@ -6424,9 +6420,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="8">
         <v>3</v>
@@ -6523,9 +6519,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" s="8">
         <v>2</v>
@@ -6622,9 +6618,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="8">
         <v>2</v>
@@ -6721,9 +6717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="8">
         <v>3</v>
@@ -6820,9 +6816,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="8">
         <v>2</v>
@@ -6919,9 +6915,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="8">
         <v>2</v>
@@ -7020,7 +7016,7 @@
     </row>
     <row r="56" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="8">
         <v>3</v>
@@ -7117,9 +7113,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="8">
         <v>3</v>
@@ -7216,9 +7212,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B58" s="8">
         <v>2</v>
@@ -7315,9 +7311,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" s="8">
         <v>1</v>
@@ -7414,9 +7410,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" s="8">
         <v>1</v>
@@ -7513,9 +7509,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" s="8">
         <v>1</v>
@@ -7612,9 +7608,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" s="8">
         <v>1</v>
@@ -7713,7 +7709,7 @@
     </row>
     <row r="63" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" s="13">
         <v>1</v>
@@ -7810,9 +7806,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" s="8">
         <v>3</v>
@@ -7909,9 +7905,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" s="8">
         <v>1</v>
@@ -8008,9 +8004,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" s="8">
         <v>2</v>
@@ -8107,9 +8103,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" s="14">
         <v>1</v>
@@ -8208,7 +8204,7 @@
     </row>
     <row r="68" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B68" s="13">
         <v>1</v>
@@ -8307,7 +8303,7 @@
     </row>
     <row r="69" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" s="8">
         <v>2</v>
@@ -8404,9 +8400,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B70" s="13">
         <v>1</v>
@@ -8503,9 +8499,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B71" s="13">
         <v>1</v>
@@ -8602,9 +8598,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B72" s="8">
         <v>1</v>
@@ -8701,9 +8697,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B73" s="13">
         <v>1</v>
@@ -8800,9 +8796,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B74" s="13">
         <v>1</v>
@@ -8899,9 +8895,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B75" s="13">
         <v>1</v>
@@ -8998,9 +8994,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B76" s="8">
         <v>2</v>
@@ -9097,9 +9093,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B77" s="8">
         <v>2</v>
@@ -9198,7 +9194,7 @@
     </row>
     <row r="78" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" s="13">
         <v>1</v>
@@ -9295,9 +9291,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" s="8">
         <v>2</v>
@@ -9394,9 +9390,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B80" s="8">
         <v>2</v>
@@ -9493,9 +9489,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B81" s="8">
         <v>3</v>
@@ -9592,9 +9588,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B82" s="8">
         <v>2</v>
@@ -9691,9 +9687,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B83" s="8">
         <v>3</v>
@@ -9790,9 +9786,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B84" s="8">
         <v>3</v>
@@ -9889,9 +9885,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" s="8">
         <v>3</v>
@@ -9988,9 +9984,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B86" s="8">
         <v>2</v>
@@ -10087,9 +10083,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:43" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:43" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B87" s="8">
         <v>3</v>
@@ -10186,9 +10182,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B88" s="8">
         <v>3</v>
@@ -10285,9 +10281,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B89" s="8">
         <v>2</v>
@@ -10384,9 +10380,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B90" s="13">
         <v>2</v>
@@ -10483,9 +10479,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B91" s="8">
         <v>1</v>
@@ -10582,9 +10578,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B92" s="8">
         <v>1</v>
@@ -10681,9 +10677,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B93" s="8">
         <v>2</v>
@@ -10780,9 +10776,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B94" s="8">
         <v>2</v>
@@ -10879,9 +10875,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B95" s="8">
         <v>1</v>
@@ -10978,9 +10974,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B96" s="8">
         <v>2</v>
@@ -11077,9 +11073,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B97" s="8">
         <v>2</v>
@@ -11176,9 +11172,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B98" s="8">
         <v>3</v>
@@ -11275,9 +11271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B99" s="8">
         <v>2</v>
@@ -11374,9 +11370,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B100" s="8">
         <v>3</v>
@@ -11473,9 +11469,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B101" s="13">
         <v>1</v>
@@ -11572,9 +11568,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:43" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:43" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B102" s="8">
         <v>3</v>
@@ -11671,9 +11667,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B103" s="8">
         <v>2</v>
@@ -11770,9 +11766,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B104" s="8">
         <v>2</v>
@@ -11871,7 +11867,7 @@
     </row>
     <row r="105" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B105" s="8">
         <v>2</v>
@@ -11970,7 +11966,7 @@
     </row>
     <row r="106" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B106" s="8">
         <v>3</v>
@@ -12067,9 +12063,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B107" s="8">
         <v>2</v>
@@ -12166,9 +12162,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B108" s="13">
         <v>2</v>
@@ -12265,9 +12261,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B109" s="8">
         <v>2</v>
@@ -12364,9 +12360,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B110" s="8">
         <v>1</v>
@@ -12463,9 +12459,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B111" s="8">
         <v>2</v>
@@ -12564,7 +12560,7 @@
     </row>
     <row r="112" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B112" s="8">
         <v>3</v>
@@ -12663,7 +12659,7 @@
     </row>
     <row r="113" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B113" s="8">
         <v>1</v>
@@ -12760,9 +12756,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B114" s="8">
         <v>1</v>
@@ -12859,9 +12855,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B115" s="8">
         <v>2</v>
@@ -12958,9 +12954,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B116" s="8">
         <v>2</v>
@@ -13057,9 +13053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B117" s="8">
         <v>3</v>
@@ -13156,9 +13152,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B118" s="8">
         <v>3</v>
@@ -13255,9 +13251,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B119" s="8">
         <v>2</v>
@@ -13354,9 +13350,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B120" s="8">
         <v>2</v>
@@ -13453,9 +13449,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B121" s="8">
         <v>3</v>
@@ -13552,9 +13548,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B122" s="8">
         <v>3</v>
@@ -13651,9 +13647,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B123" s="8">
         <v>3</v>
@@ -13750,9 +13746,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B124" s="8">
         <v>3</v>
@@ -13849,9 +13845,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B125" s="13">
         <v>1</v>
@@ -13948,9 +13944,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B126" s="8">
         <v>3</v>
@@ -14047,9 +14043,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B127" s="8">
         <v>1</v>
@@ -14146,9 +14142,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B128" s="8">
         <v>2</v>
@@ -14245,9 +14241,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B129" s="8">
         <v>3</v>
@@ -14344,9 +14340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B130" s="8">
         <v>2</v>
@@ -14443,9 +14439,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B131" s="8">
         <v>2</v>
@@ -14544,7 +14540,7 @@
     </row>
     <row r="132" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A132" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B132" s="13">
         <v>1</v>
@@ -14641,9 +14637,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B133" s="8">
         <v>3</v>
@@ -14740,9 +14736,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B134" s="8">
         <v>2</v>
@@ -14839,9 +14835,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B135" s="8">
         <v>1</v>
@@ -14940,7 +14936,7 @@
     </row>
     <row r="136" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B136" s="8">
         <v>2</v>
@@ -15037,9 +15033,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B137" s="8">
         <v>3</v>
@@ -15136,9 +15132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B138" s="13">
         <v>1</v>
@@ -15235,9 +15231,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B139" s="8">
         <v>2</v>
@@ -15334,9 +15330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B140" s="13">
         <v>1</v>
@@ -15433,9 +15429,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B141" s="8">
         <v>2</v>
@@ -15532,9 +15528,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B142" s="8">
         <v>1</v>
@@ -15631,9 +15627,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B143" s="8">
         <v>2</v>
@@ -15730,9 +15726,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B144" s="8">
         <v>2</v>
@@ -15829,9 +15825,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B145" s="8">
         <v>2</v>
@@ -15930,7 +15926,7 @@
     </row>
     <row r="146" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A146" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B146" s="8">
         <v>2</v>
@@ -16027,9 +16023,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B147" s="8">
         <v>2</v>
@@ -16126,9 +16122,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A148" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B148" s="13">
         <v>2</v>
@@ -16225,9 +16221,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B149" s="8">
         <v>1</v>
@@ -16324,9 +16320,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B150" s="8">
         <v>2</v>
@@ -16423,9 +16419,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B151" s="8">
         <v>1</v>
@@ -16522,9 +16518,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B152" s="8">
         <v>2</v>
@@ -16621,9 +16617,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B153" s="8">
         <v>3</v>
@@ -16720,9 +16716,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B154" s="8">
         <v>2</v>
@@ -16819,9 +16815,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B155" s="8">
         <v>3</v>
@@ -16918,9 +16914,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B156" s="8">
         <v>3</v>
@@ -17017,9 +17013,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A157" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B157" s="13">
         <v>2</v>
@@ -17116,9 +17112,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A158" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B158" s="8">
         <v>1</v>
@@ -17215,9 +17211,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A159" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B159" s="13">
         <v>2</v>
@@ -17316,7 +17312,7 @@
     </row>
     <row r="160" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B160" s="13">
         <v>1</v>
@@ -17413,9 +17409,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B161" s="8">
         <v>3</v>
@@ -17512,9 +17508,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A162" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B162" s="8">
         <v>3</v>
@@ -17611,9 +17607,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B163" s="8">
         <v>3</v>
@@ -17710,9 +17706,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A164" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B164" s="8">
         <v>3</v>
@@ -17809,9 +17805,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B165" s="8">
         <v>3</v>
@@ -17908,9 +17904,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A166" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B166" s="8">
         <v>2</v>
@@ -18007,9 +18003,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B167" s="8">
         <v>3</v>
@@ -18106,9 +18102,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A168" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B168" s="8">
         <v>3</v>
@@ -18205,9 +18201,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B169" s="8">
         <v>1</v>
@@ -18306,7 +18302,7 @@
     </row>
     <row r="170" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A170" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B170" s="13">
         <v>1</v>
@@ -18405,7 +18401,7 @@
     </row>
     <row r="171" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A171" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B171" s="13">
         <v>1</v>
@@ -18502,9 +18498,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A172" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B172" s="8">
         <v>2</v>
@@ -18601,9 +18597,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B173" s="8">
         <v>2</v>
@@ -18700,9 +18696,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A174" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B174" s="8">
         <v>2</v>
@@ -18799,9 +18795,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B175" s="8">
         <v>3</v>
@@ -18898,9 +18894,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A176" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B176" s="8">
         <v>2</v>
@@ -18997,9 +18993,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B177" s="8">
         <v>1</v>
@@ -19096,9 +19092,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A178" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B178" s="8">
         <v>3</v>
@@ -19195,9 +19191,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B179" s="8">
         <v>1</v>
@@ -19294,9 +19290,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A180" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B180" s="8">
         <v>1</v>
@@ -19393,9 +19389,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B181" s="8">
         <v>3</v>
@@ -19494,7 +19490,7 @@
     </row>
     <row r="182" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A182" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B182" s="13">
         <v>1</v>
@@ -19591,9 +19587,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B183" s="8">
         <v>3</v>
@@ -19690,9 +19686,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A184" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B184" s="8">
         <v>2</v>
@@ -19791,7 +19787,7 @@
     </row>
     <row r="185" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B185" s="8">
         <v>3</v>
@@ -19888,9 +19884,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B186" s="8">
         <v>3</v>
@@ -19987,9 +19983,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B187" s="8">
         <v>1</v>
@@ -20086,9 +20082,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A188" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B188" s="8">
         <v>3</v>
@@ -20185,9 +20181,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:43" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B189" s="8">
         <v>3</v>
@@ -20286,7 +20282,7 @@
     </row>
     <row r="190" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A190" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B190" s="8">
         <v>2</v>
@@ -20385,37 +20381,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AR190" xr:uid="{4E863BDD-F346-1648-BFCC-763B278D18B9}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Adonis annua"/>
-        <filter val="Alyssum alyssoides"/>
-        <filter val="Anthriscus caucalis"/>
-        <filter val="Aphenes arvensis"/>
-        <filter val="Atriplex prostrata"/>
-        <filter val="Centaurea cyanus"/>
-        <filter val="Chamaenerion angustifolium"/>
-        <filter val="Chrysanthemum segetum"/>
-        <filter val="Epilobium montanum"/>
-        <filter val="Euphorbia platyphyllos"/>
-        <filter val="Filago pyramidata"/>
-        <filter val="Filago vulgaris"/>
-        <filter val="Galium tricornutum"/>
-        <filter val="Medicago arabica"/>
-        <filter val="Medicago lupilina"/>
-        <filter val="Odontites verna"/>
-        <filter val="Papaver dubium"/>
-        <filter val="Scandix pecten-veneris"/>
-        <filter val="Sherardia arvensis"/>
-        <filter val="Sonchus arvensis"/>
-        <filter val="Species"/>
-        <filter val="Torilis arvensis"/>
-        <filter val="Valerianella dentata"/>
-        <filter val="Valerianella rimosa"/>
-        <filter val="Veronica triphyllos"/>
-        <filter val="Vicia sativa"/>
-        <filter val="Viola tricolor"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
@@ -20465,10 +20430,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" t="s">
         <v>220</v>
-      </c>
-      <c r="B1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20476,7 +20441,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20484,7 +20449,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20492,7 +20457,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20500,7 +20465,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20508,7 +20473,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20516,7 +20481,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20524,7 +20489,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20532,7 +20497,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20540,7 +20505,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20548,7 +20513,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20556,7 +20521,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20564,7 +20529,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20572,7 +20537,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20580,7 +20545,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20588,7 +20553,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20596,7 +20561,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20604,7 +20569,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20612,7 +20577,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20620,7 +20585,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20628,7 +20593,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20636,7 +20601,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20644,7 +20609,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20652,7 +20617,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -20660,7 +20625,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -20668,7 +20633,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -20676,7 +20641,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -20684,7 +20649,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -20692,7 +20657,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -20700,7 +20665,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -20708,7 +20673,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fill in moisture and nitrogen rows for geranium pusillum and malva sylvestris, change alyssum alyssoides ellenburg moisture score to 5
</commit_message>
<xml_diff>
--- a/Arable_plant_requirements.xlsx
+++ b/Arable_plant_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC331908-EA0F-FE41-A027-3511153566F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA1C263-3C58-1946-B684-236F0EA7F9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1080,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1232,6 +1232,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1574,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK163" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AT9" sqref="AT9"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2559,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="AT9" s="64">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AU9" s="11"/>
     </row>
@@ -10275,12 +10278,24 @@
       <c r="AG82" s="9">
         <v>1</v>
       </c>
-      <c r="AJ82" s="30"/>
-      <c r="AK82" s="11"/>
-      <c r="AL82" s="11"/>
-      <c r="AO82" s="30"/>
-      <c r="AP82" s="11"/>
-      <c r="AQ82" s="11"/>
+      <c r="AJ82" s="65">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="64">
+        <v>1</v>
+      </c>
+      <c r="AL82" s="64">
+        <v>1</v>
+      </c>
+      <c r="AO82" s="65">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="64">
+        <v>1</v>
+      </c>
+      <c r="AQ82" s="64">
+        <v>1</v>
+      </c>
       <c r="AS82" s="11">
         <v>7</v>
       </c>
@@ -12595,12 +12610,24 @@
       <c r="AG104" s="9">
         <v>0</v>
       </c>
-      <c r="AJ104" s="30"/>
-      <c r="AK104" s="11"/>
-      <c r="AL104" s="11"/>
-      <c r="AO104" s="30"/>
-      <c r="AP104" s="11"/>
-      <c r="AQ104" s="11"/>
+      <c r="AJ104" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK104" s="64">
+        <v>0</v>
+      </c>
+      <c r="AL104" s="64">
+        <v>0</v>
+      </c>
+      <c r="AO104" s="65">
+        <v>1</v>
+      </c>
+      <c r="AP104" s="64">
+        <v>0</v>
+      </c>
+      <c r="AQ104" s="64">
+        <v>0</v>
+      </c>
       <c r="AS104" s="11">
         <v>7</v>
       </c>

</xml_diff>